<commit_message>
IMPLEMENTASI JS-08 PRAKTIKUM 1: Implementasi Upload File untuk import data (Penjualan)✨
</commit_message>
<xml_diff>
--- a/POS/public/template_stok.xlsx
+++ b/POS/public/template_stok.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F254E4-4E44-4F78-90A5-9B980419189A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7575FF3B-EF64-453F-848D-40F7AFF77A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15960" yWindow="263" windowWidth="16200" windowHeight="9359" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>supplier_id</t>
   </si>
@@ -439,21 +439,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.46484375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,12 +470,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -487,12 +487,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -502,23 +502,6 @@
       </c>
       <c r="E3">
         <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>